<commit_message>
Sutvarkytas studento saugojimo vietos atmintyje išvedimas
</commit_message>
<xml_diff>
--- a/programos-spartos-analize.xlsx
+++ b/programos-spartos-analize.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mykolasmotiejunas/Documents/vs-git-repositories/objektinis-pirma/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E96137E0-D7DB-6144-B544-C81908B33EB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC89BE5D-D54B-FF42-824F-853E7F2E329F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16220" xr2:uid="{AEA47B78-08EF-3743-9352-70FFE0876222}"/>
   </bookViews>
@@ -455,7 +455,7 @@
   <dimension ref="B2:N11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
README.md papildytas programos spartos analize naudojant 1, 2 ir 3 strategijas
</commit_message>
<xml_diff>
--- a/programos-spartos-analize.xlsx
+++ b/programos-spartos-analize.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11027"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mykolasmotiejunas/Documents/vs-git-repositories/objektinis-pirma/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC89BE5D-D54B-FF42-824F-853E7F2E329F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{748A8FCC-74BF-764F-9C81-ECA1EDEB9CD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16220" xr2:uid="{AEA47B78-08EF-3743-9352-70FFE0876222}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="15">
   <si>
     <t>std::vector</t>
   </si>
@@ -66,6 +66,21 @@
   </si>
   <si>
     <t>Bendras veikimo laikas be generavimo</t>
+  </si>
+  <si>
+    <t>1 strategija</t>
+  </si>
+  <si>
+    <t>2 strategija</t>
+  </si>
+  <si>
+    <t>3 strategija</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Pastaba: "-" žymi, kad programa veikė ilgiau nei 40 min</t>
   </si>
 </sst>
 </file>
@@ -108,13 +123,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -452,10 +466,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BB18AB8-3974-C64F-83B9-2240ECB77FEA}">
-  <dimension ref="B2:N11"/>
+  <dimension ref="D6:N58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="M61" sqref="M61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -465,326 +479,1237 @@
     <col min="14" max="14" width="36" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="D2" s="1" t="s">
+    <row r="6" spans="4:14" x14ac:dyDescent="0.2">
+      <c r="D6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
-    </row>
-    <row r="3" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B3" s="2"/>
-      <c r="D3" s="4">
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+    </row>
+    <row r="7" spans="4:14" x14ac:dyDescent="0.2">
+      <c r="D7" s="3">
         <v>1000</v>
       </c>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4">
+      <c r="E7" s="3"/>
+      <c r="F7" s="3">
         <v>10000</v>
       </c>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4">
+      <c r="G7" s="3"/>
+      <c r="H7" s="3">
         <v>100000</v>
       </c>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4">
+      <c r="I7" s="3"/>
+      <c r="J7" s="3">
         <v>1000000</v>
       </c>
-      <c r="K3" s="4"/>
-      <c r="L3" s="4">
+      <c r="K7" s="3"/>
+      <c r="L7" s="3">
         <v>10000000</v>
       </c>
-      <c r="M3" s="4"/>
-    </row>
-    <row r="4" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="D4" s="1">
+      <c r="M7" s="3"/>
+    </row>
+    <row r="8" spans="4:14" x14ac:dyDescent="0.2">
+      <c r="D8" s="2">
         <v>6.9681300000000003E-3</v>
       </c>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1">
+      <c r="E8" s="2"/>
+      <c r="F8" s="2">
         <v>4.7327800000000003E-2</v>
       </c>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1">
+      <c r="G8" s="2"/>
+      <c r="H8" s="2">
         <v>0.24769099999999999</v>
       </c>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1">
+      <c r="I8" s="2"/>
+      <c r="J8" s="2">
         <v>1.9952700000000001</v>
       </c>
-      <c r="K4" s="1"/>
-      <c r="L4" s="1">
+      <c r="K8" s="2"/>
+      <c r="L8" s="2">
         <v>18.982700000000001</v>
       </c>
-      <c r="M4" s="1"/>
-      <c r="N4" s="2" t="s">
+      <c r="M8" s="2"/>
+      <c r="N8" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="D5" t="s">
-        <v>0</v>
-      </c>
-      <c r="E5" t="s">
-        <v>1</v>
-      </c>
-      <c r="F5" t="s">
-        <v>0</v>
-      </c>
-      <c r="G5" t="s">
-        <v>1</v>
-      </c>
-      <c r="H5" t="s">
-        <v>0</v>
-      </c>
-      <c r="I5" t="s">
-        <v>1</v>
-      </c>
-      <c r="J5" t="s">
-        <v>0</v>
-      </c>
-      <c r="K5" t="s">
-        <v>1</v>
-      </c>
-      <c r="L5" t="s">
-        <v>0</v>
-      </c>
-      <c r="M5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="D6">
+    <row r="9" spans="4:14" x14ac:dyDescent="0.2">
+      <c r="D9" t="s">
+        <v>0</v>
+      </c>
+      <c r="E9" t="s">
+        <v>1</v>
+      </c>
+      <c r="F9" t="s">
+        <v>0</v>
+      </c>
+      <c r="G9" t="s">
+        <v>1</v>
+      </c>
+      <c r="H9" t="s">
+        <v>0</v>
+      </c>
+      <c r="I9" t="s">
+        <v>1</v>
+      </c>
+      <c r="J9" t="s">
+        <v>0</v>
+      </c>
+      <c r="K9" t="s">
+        <v>1</v>
+      </c>
+      <c r="L9" t="s">
+        <v>0</v>
+      </c>
+      <c r="M9" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="4:14" x14ac:dyDescent="0.2">
+      <c r="D10">
         <v>9.2629600000000006E-3</v>
       </c>
-      <c r="E6">
+      <c r="E10">
         <v>6.0172100000000003E-3</v>
       </c>
-      <c r="F6">
+      <c r="F10">
         <v>5.2518299999999997E-2</v>
       </c>
-      <c r="G6">
+      <c r="G10">
         <v>2.33253E-2</v>
       </c>
-      <c r="H6">
+      <c r="H10">
         <v>0.26019799999999998</v>
       </c>
-      <c r="I6">
+      <c r="I10">
         <v>0.21951499999999999</v>
       </c>
-      <c r="J6">
+      <c r="J10">
         <v>2.2223600000000001</v>
       </c>
-      <c r="K6">
+      <c r="K10">
         <v>2.1867999999999999</v>
       </c>
-      <c r="L6">
+      <c r="L10">
         <v>23.3002</v>
       </c>
-      <c r="M6">
+      <c r="M10">
         <v>22.782299999999999</v>
       </c>
-      <c r="N6" t="s">
+      <c r="N10" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="D7">
+    <row r="11" spans="4:14" x14ac:dyDescent="0.2">
+      <c r="D11">
         <v>1.9525E-4</v>
       </c>
-      <c r="E7">
+      <c r="E11">
         <v>1.47083E-4</v>
       </c>
-      <c r="F7">
+      <c r="F11">
         <v>1.02446E-3</v>
       </c>
-      <c r="G7">
+      <c r="G11">
         <v>1.1088300000000001E-3</v>
       </c>
-      <c r="H7">
+      <c r="H11">
         <v>6.3495799999999996E-3</v>
       </c>
-      <c r="I7">
+      <c r="I11">
         <v>3.0816699999999999E-2</v>
       </c>
-      <c r="J7">
+      <c r="J11">
         <v>6.5535899999999994E-2</v>
       </c>
-      <c r="K7">
+      <c r="K11">
         <v>0.68362299999999998</v>
       </c>
-      <c r="L7">
+      <c r="L11">
         <v>0.90573199999999998</v>
       </c>
-      <c r="M7">
+      <c r="M11">
         <v>12.101699999999999</v>
       </c>
-      <c r="N7" t="s">
+      <c r="N11" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="D8">
+    <row r="12" spans="4:14" x14ac:dyDescent="0.2">
+      <c r="D12">
         <v>5.11292E-4</v>
       </c>
-      <c r="E8">
+      <c r="E12">
         <v>4.6558400000000001E-4</v>
       </c>
-      <c r="F8">
+      <c r="F12">
         <v>2.6779199999999999E-3</v>
       </c>
-      <c r="G8">
+      <c r="G12">
         <v>1.89529E-3</v>
       </c>
-      <c r="H8">
+      <c r="H12">
         <v>2.4851999999999999E-2</v>
       </c>
-      <c r="I8">
+      <c r="I12">
         <v>3.84334E-2</v>
       </c>
-      <c r="J8">
+      <c r="J12">
         <v>0.36590299999999998</v>
       </c>
-      <c r="K8">
+      <c r="K12">
         <v>0.544798</v>
       </c>
-      <c r="L8">
+      <c r="L12">
         <v>10.3277</v>
       </c>
-      <c r="M8">
+      <c r="M12">
         <v>74.269199999999998</v>
       </c>
-      <c r="N8" t="s">
+      <c r="N12" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="D9">
+    <row r="13" spans="4:14" x14ac:dyDescent="0.2">
+      <c r="D13">
         <v>4.8587500000000002E-3</v>
       </c>
-      <c r="E9">
+      <c r="E13">
         <v>3.23946E-3</v>
       </c>
-      <c r="F9">
+      <c r="F13">
         <v>1.86727E-2</v>
       </c>
-      <c r="G9">
+      <c r="G13">
         <v>1.34973E-2</v>
       </c>
-      <c r="H9">
+      <c r="H13">
         <v>0.128943</v>
       </c>
-      <c r="I9">
+      <c r="I13">
         <v>0.13794600000000001</v>
       </c>
-      <c r="J9">
+      <c r="J13">
         <v>1.3740399999999999</v>
       </c>
-      <c r="K9">
+      <c r="K13">
         <v>1.3433600000000001</v>
       </c>
-      <c r="L9">
+      <c r="L13">
         <v>13.986800000000001</v>
       </c>
-      <c r="M9">
+      <c r="M13">
         <v>14.523</v>
       </c>
-      <c r="N9" s="3" t="s">
+      <c r="N13" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="D10">
+    <row r="14" spans="4:14" x14ac:dyDescent="0.2">
+      <c r="D14">
         <v>4.0812899999999996E-3</v>
       </c>
-      <c r="E10">
+      <c r="E14">
         <v>3.3087099999999999E-3</v>
       </c>
-      <c r="F10">
+      <c r="F14">
         <v>1.54272E-2</v>
       </c>
-      <c r="G10">
+      <c r="G14">
         <v>1.30723E-2</v>
       </c>
-      <c r="H10">
+      <c r="H14">
         <v>0.12712399999999999</v>
       </c>
-      <c r="I10">
+      <c r="I14">
         <v>0.13253400000000001</v>
       </c>
-      <c r="J10">
+      <c r="J14">
         <v>1.3329</v>
       </c>
-      <c r="K10">
+      <c r="K14">
         <v>1.30647</v>
       </c>
-      <c r="L10">
+      <c r="L14">
         <v>15.6075</v>
       </c>
-      <c r="M10">
+      <c r="M14">
         <v>14.542899999999999</v>
       </c>
-      <c r="N10" s="3" t="s">
+      <c r="N14" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="D11">
+    <row r="15" spans="4:14" x14ac:dyDescent="0.2">
+      <c r="D15">
         <v>1.8966500000000001E-2</v>
       </c>
-      <c r="E11">
+      <c r="E15">
         <v>1.3226999999999999E-2</v>
       </c>
-      <c r="F11">
+      <c r="F15">
         <v>9.0366000000000002E-2</v>
       </c>
-      <c r="G11">
+      <c r="G15">
         <v>5.2938699999999998E-2</v>
       </c>
-      <c r="H11">
+      <c r="H15">
         <v>0.54753600000000002</v>
       </c>
-      <c r="I11">
+      <c r="I15">
         <v>0.55931500000000001</v>
       </c>
-      <c r="J11">
+      <c r="J15">
         <v>5.3608200000000004</v>
       </c>
-      <c r="K11">
+      <c r="K15">
         <v>6.0651299999999999</v>
       </c>
-      <c r="L11">
+      <c r="L15">
         <v>64.128</v>
       </c>
-      <c r="M11">
+      <c r="M15">
         <v>138.21899999999999</v>
       </c>
-      <c r="N11" t="s">
+      <c r="N15" t="s">
         <v>9</v>
       </c>
     </row>
+    <row r="23" spans="4:14" x14ac:dyDescent="0.2">
+      <c r="D23" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
+      <c r="H23" s="3"/>
+      <c r="I23" s="3"/>
+      <c r="J23" s="3"/>
+      <c r="K23" s="3"/>
+      <c r="L23" s="3"/>
+      <c r="M23" s="3"/>
+    </row>
+    <row r="24" spans="4:14" x14ac:dyDescent="0.2">
+      <c r="D24" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
+      <c r="I24" s="2"/>
+      <c r="J24" s="2"/>
+      <c r="K24" s="2"/>
+      <c r="L24" s="2"/>
+      <c r="M24" s="2"/>
+    </row>
+    <row r="25" spans="4:14" x14ac:dyDescent="0.2">
+      <c r="D25" s="3">
+        <v>1000</v>
+      </c>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3">
+        <v>10000</v>
+      </c>
+      <c r="G25" s="3"/>
+      <c r="H25" s="3">
+        <v>100000</v>
+      </c>
+      <c r="I25" s="3"/>
+      <c r="J25" s="3">
+        <v>1000000</v>
+      </c>
+      <c r="K25" s="3"/>
+      <c r="L25" s="3">
+        <v>10000000</v>
+      </c>
+      <c r="M25" s="3"/>
+    </row>
+    <row r="26" spans="4:14" x14ac:dyDescent="0.2">
+      <c r="D26" t="s">
+        <v>0</v>
+      </c>
+      <c r="E26" t="s">
+        <v>1</v>
+      </c>
+      <c r="F26" t="s">
+        <v>0</v>
+      </c>
+      <c r="G26" t="s">
+        <v>1</v>
+      </c>
+      <c r="H26" t="s">
+        <v>0</v>
+      </c>
+      <c r="I26" t="s">
+        <v>1</v>
+      </c>
+      <c r="J26" t="s">
+        <v>0</v>
+      </c>
+      <c r="K26" t="s">
+        <v>1</v>
+      </c>
+      <c r="L26" t="s">
+        <v>0</v>
+      </c>
+      <c r="M26" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="4:14" x14ac:dyDescent="0.2">
+      <c r="D27">
+        <v>6.1942500000000001E-3</v>
+      </c>
+      <c r="E27">
+        <v>4.4885000000000003E-3</v>
+      </c>
+      <c r="F27">
+        <v>3.01014E-2</v>
+      </c>
+      <c r="G27">
+        <v>2.31922E-2</v>
+      </c>
+      <c r="H27">
+        <v>0.26572000000000001</v>
+      </c>
+      <c r="I27">
+        <v>0.239977</v>
+      </c>
+      <c r="J27">
+        <v>2.2955000000000001</v>
+      </c>
+      <c r="K27">
+        <v>2.2295799999999999</v>
+      </c>
+      <c r="L27">
+        <v>25.444800000000001</v>
+      </c>
+      <c r="M27">
+        <v>23.340499999999999</v>
+      </c>
+      <c r="N27" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="4:14" x14ac:dyDescent="0.2">
+      <c r="D28">
+        <v>1.20209E-4</v>
+      </c>
+      <c r="E28">
+        <v>1.10917E-4</v>
+      </c>
+      <c r="F28">
+        <v>6.6387499999999997E-4</v>
+      </c>
+      <c r="G28">
+        <v>1.6973299999999999E-3</v>
+      </c>
+      <c r="H28">
+        <v>6.8089200000000004E-3</v>
+      </c>
+      <c r="I28">
+        <v>3.6743499999999998E-2</v>
+      </c>
+      <c r="J28">
+        <v>0.101106</v>
+      </c>
+      <c r="K28">
+        <v>0.84311800000000003</v>
+      </c>
+      <c r="L28">
+        <v>0.90696299999999996</v>
+      </c>
+      <c r="M28">
+        <v>22.118600000000001</v>
+      </c>
+      <c r="N28" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="4:14" x14ac:dyDescent="0.2">
+      <c r="D29">
+        <v>2.8983399999999999E-4</v>
+      </c>
+      <c r="E29">
+        <v>3.19792E-4</v>
+      </c>
+      <c r="F29">
+        <v>1.6764200000000001E-3</v>
+      </c>
+      <c r="G29">
+        <v>2.0855399999999999E-3</v>
+      </c>
+      <c r="H29">
+        <v>2.9169E-2</v>
+      </c>
+      <c r="I29">
+        <v>4.8246600000000001E-2</v>
+      </c>
+      <c r="J29">
+        <v>0.42185400000000001</v>
+      </c>
+      <c r="K29">
+        <v>0.57590300000000005</v>
+      </c>
+      <c r="L29">
+        <v>26.700700000000001</v>
+      </c>
+      <c r="M29">
+        <v>130.083</v>
+      </c>
+      <c r="N29" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="4:14" x14ac:dyDescent="0.2">
+      <c r="D30">
+        <v>2.73529E-3</v>
+      </c>
+      <c r="E30">
+        <v>2.4671699999999999E-3</v>
+      </c>
+      <c r="F30">
+        <v>1.6187699999999999E-2</v>
+      </c>
+      <c r="G30">
+        <v>1.82089E-2</v>
+      </c>
+      <c r="H30">
+        <v>0.13806499999999999</v>
+      </c>
+      <c r="I30">
+        <v>0.144649</v>
+      </c>
+      <c r="J30">
+        <v>1.5667899999999999</v>
+      </c>
+      <c r="K30">
+        <v>1.4005399999999999</v>
+      </c>
+      <c r="L30">
+        <v>15.003399999999999</v>
+      </c>
+      <c r="M30">
+        <v>15.4099</v>
+      </c>
+      <c r="N30" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="4:14" x14ac:dyDescent="0.2">
+      <c r="D31">
+        <v>2.8202100000000001E-3</v>
+      </c>
+      <c r="E31">
+        <v>2.1871199999999999E-3</v>
+      </c>
+      <c r="F31">
+        <v>1.9031900000000001E-2</v>
+      </c>
+      <c r="G31">
+        <v>1.50642E-2</v>
+      </c>
+      <c r="H31">
+        <v>0.134238</v>
+      </c>
+      <c r="I31">
+        <v>0.144785</v>
+      </c>
+      <c r="J31">
+        <v>1.45133</v>
+      </c>
+      <c r="K31">
+        <v>1.3559000000000001</v>
+      </c>
+      <c r="L31">
+        <v>14.518700000000001</v>
+      </c>
+      <c r="M31">
+        <v>15.7272</v>
+      </c>
+      <c r="N31" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="32" spans="4:14" x14ac:dyDescent="0.2">
+      <c r="D32">
+        <v>1.2203500000000001E-2</v>
+      </c>
+      <c r="E32">
+        <v>9.6102500000000007E-3</v>
+      </c>
+      <c r="F32">
+        <v>6.7709000000000005E-2</v>
+      </c>
+      <c r="G32">
+        <v>6.0303799999999998E-2</v>
+      </c>
+      <c r="H32">
+        <v>0.57408400000000004</v>
+      </c>
+      <c r="I32">
+        <v>0.61448199999999997</v>
+      </c>
+      <c r="J32">
+        <v>5.8366899999999999</v>
+      </c>
+      <c r="K32">
+        <v>6.4051400000000003</v>
+      </c>
+      <c r="L32">
+        <v>82.575199999999995</v>
+      </c>
+      <c r="M32">
+        <v>206.68</v>
+      </c>
+      <c r="N32" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="36" spans="4:14" x14ac:dyDescent="0.2">
+      <c r="D36" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E36" s="3"/>
+      <c r="F36" s="3"/>
+      <c r="G36" s="3"/>
+      <c r="H36" s="3"/>
+      <c r="I36" s="3"/>
+      <c r="J36" s="3"/>
+      <c r="K36" s="3"/>
+      <c r="L36" s="3"/>
+      <c r="M36" s="3"/>
+    </row>
+    <row r="37" spans="4:14" x14ac:dyDescent="0.2">
+      <c r="D37" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E37" s="2"/>
+      <c r="F37" s="2"/>
+      <c r="G37" s="2"/>
+      <c r="H37" s="2"/>
+      <c r="I37" s="2"/>
+      <c r="J37" s="2"/>
+      <c r="K37" s="2"/>
+      <c r="L37" s="2"/>
+      <c r="M37" s="2"/>
+    </row>
+    <row r="38" spans="4:14" x14ac:dyDescent="0.2">
+      <c r="D38" s="3">
+        <v>1000</v>
+      </c>
+      <c r="E38" s="3"/>
+      <c r="F38" s="3">
+        <v>10000</v>
+      </c>
+      <c r="G38" s="3"/>
+      <c r="H38" s="3">
+        <v>100000</v>
+      </c>
+      <c r="I38" s="3"/>
+      <c r="J38" s="3">
+        <v>1000000</v>
+      </c>
+      <c r="K38" s="3"/>
+      <c r="L38" s="3">
+        <v>10000000</v>
+      </c>
+      <c r="M38" s="3"/>
+    </row>
+    <row r="39" spans="4:14" x14ac:dyDescent="0.2">
+      <c r="D39" t="s">
+        <v>0</v>
+      </c>
+      <c r="E39" t="s">
+        <v>1</v>
+      </c>
+      <c r="F39" t="s">
+        <v>0</v>
+      </c>
+      <c r="G39" t="s">
+        <v>1</v>
+      </c>
+      <c r="H39" t="s">
+        <v>0</v>
+      </c>
+      <c r="I39" t="s">
+        <v>1</v>
+      </c>
+      <c r="J39" t="s">
+        <v>0</v>
+      </c>
+      <c r="K39" t="s">
+        <v>1</v>
+      </c>
+      <c r="L39" t="s">
+        <v>0</v>
+      </c>
+      <c r="M39" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="4:14" x14ac:dyDescent="0.2">
+      <c r="D40">
+        <v>9.6822100000000001E-3</v>
+      </c>
+      <c r="E40">
+        <v>6.1026700000000001E-3</v>
+      </c>
+      <c r="F40">
+        <v>5.3296000000000003E-2</v>
+      </c>
+      <c r="G40">
+        <v>2.2137899999999999E-2</v>
+      </c>
+      <c r="H40">
+        <v>0.26466600000000001</v>
+      </c>
+      <c r="I40">
+        <v>0.22304299999999999</v>
+      </c>
+      <c r="J40">
+        <v>2.2208700000000001</v>
+      </c>
+      <c r="K40">
+        <v>2.30375</v>
+      </c>
+      <c r="L40">
+        <v>24.819800000000001</v>
+      </c>
+      <c r="M40">
+        <v>23.026900000000001</v>
+      </c>
+      <c r="N40" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="4:14" x14ac:dyDescent="0.2">
+      <c r="D41">
+        <v>1.96083E-4</v>
+      </c>
+      <c r="E41">
+        <v>1.56334E-4</v>
+      </c>
+      <c r="F41">
+        <v>1.03921E-3</v>
+      </c>
+      <c r="G41">
+        <v>1.01833E-3</v>
+      </c>
+      <c r="H41">
+        <v>6.2238299999999996E-3</v>
+      </c>
+      <c r="I41">
+        <v>3.2417700000000001E-2</v>
+      </c>
+      <c r="J41">
+        <v>6.8279999999999993E-2</v>
+      </c>
+      <c r="K41">
+        <v>0.76752100000000001</v>
+      </c>
+      <c r="L41">
+        <v>0.951322</v>
+      </c>
+      <c r="M41">
+        <v>38.767800000000001</v>
+      </c>
+      <c r="N41" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" spans="4:14" x14ac:dyDescent="0.2">
+      <c r="D42">
+        <v>1.7502100000000001E-3</v>
+      </c>
+      <c r="E42">
+        <v>1.7729200000000001E-4</v>
+      </c>
+      <c r="F42">
+        <v>6.6241700000000001E-2</v>
+      </c>
+      <c r="G42">
+        <v>6.8370799999999999E-4</v>
+      </c>
+      <c r="H42">
+        <v>5.6047700000000003</v>
+      </c>
+      <c r="I42">
+        <v>2.54617E-2</v>
+      </c>
+      <c r="J42" t="s">
+        <v>13</v>
+      </c>
+      <c r="K42">
+        <v>0.28170299999999998</v>
+      </c>
+      <c r="L42" t="s">
+        <v>13</v>
+      </c>
+      <c r="M42">
+        <v>32.947699999999998</v>
+      </c>
+      <c r="N42" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="43" spans="4:14" x14ac:dyDescent="0.2">
+      <c r="D43">
+        <v>4.6715799999999998E-3</v>
+      </c>
+      <c r="E43">
+        <v>3.4388299999999999E-3</v>
+      </c>
+      <c r="F43">
+        <v>1.49216E-2</v>
+      </c>
+      <c r="G43">
+        <v>1.3551499999999999E-2</v>
+      </c>
+      <c r="H43">
+        <v>0.141679</v>
+      </c>
+      <c r="I43">
+        <v>0.14622199999999999</v>
+      </c>
+      <c r="J43" t="s">
+        <v>13</v>
+      </c>
+      <c r="K43">
+        <v>1.56711</v>
+      </c>
+      <c r="L43" t="s">
+        <v>13</v>
+      </c>
+      <c r="M43">
+        <v>59.392099999999999</v>
+      </c>
+      <c r="N43" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="44" spans="4:14" x14ac:dyDescent="0.2">
+      <c r="D44">
+        <v>3.8772899999999998E-3</v>
+      </c>
+      <c r="E44">
+        <v>2.9432500000000001E-3</v>
+      </c>
+      <c r="F44">
+        <v>1.4386599999999999E-2</v>
+      </c>
+      <c r="G44">
+        <v>1.3868800000000001E-2</v>
+      </c>
+      <c r="H44">
+        <v>0.13297600000000001</v>
+      </c>
+      <c r="I44">
+        <v>0.14013400000000001</v>
+      </c>
+      <c r="J44" t="s">
+        <v>13</v>
+      </c>
+      <c r="K44">
+        <v>1.41126</v>
+      </c>
+      <c r="L44" t="s">
+        <v>13</v>
+      </c>
+      <c r="M44">
+        <v>42.456299999999999</v>
+      </c>
+      <c r="N44" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="45" spans="4:14" x14ac:dyDescent="0.2">
+      <c r="D45">
+        <v>2.0249199999999998E-2</v>
+      </c>
+      <c r="E45">
+        <v>1.28577E-2</v>
+      </c>
+      <c r="F45">
+        <v>0.149949</v>
+      </c>
+      <c r="G45">
+        <v>5.1294800000000002E-2</v>
+      </c>
+      <c r="H45">
+        <v>6.1503899999999998</v>
+      </c>
+      <c r="I45">
+        <v>0.56735199999999997</v>
+      </c>
+      <c r="J45" t="s">
+        <v>13</v>
+      </c>
+      <c r="K45">
+        <v>6.3314599999999999</v>
+      </c>
+      <c r="L45" t="s">
+        <v>13</v>
+      </c>
+      <c r="M45">
+        <v>196.59100000000001</v>
+      </c>
+      <c r="N45" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="46" spans="4:14" x14ac:dyDescent="0.2">
+      <c r="D46" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E46" s="2"/>
+      <c r="F46" s="2"/>
+      <c r="G46" s="2"/>
+      <c r="H46" s="2"/>
+      <c r="I46" s="2"/>
+      <c r="J46" s="2"/>
+      <c r="K46" s="2"/>
+      <c r="L46" s="2"/>
+      <c r="M46" s="2"/>
+    </row>
+    <row r="49" spans="4:14" x14ac:dyDescent="0.2">
+      <c r="D49" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E49" s="3"/>
+      <c r="F49" s="3"/>
+      <c r="G49" s="3"/>
+      <c r="H49" s="3"/>
+      <c r="I49" s="3"/>
+      <c r="J49" s="3"/>
+      <c r="K49" s="3"/>
+      <c r="L49" s="3"/>
+      <c r="M49" s="3"/>
+    </row>
+    <row r="50" spans="4:14" x14ac:dyDescent="0.2">
+      <c r="D50" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E50" s="2"/>
+      <c r="F50" s="2"/>
+      <c r="G50" s="2"/>
+      <c r="H50" s="2"/>
+      <c r="I50" s="2"/>
+      <c r="J50" s="2"/>
+      <c r="K50" s="2"/>
+      <c r="L50" s="2"/>
+      <c r="M50" s="2"/>
+    </row>
+    <row r="51" spans="4:14" x14ac:dyDescent="0.2">
+      <c r="D51" s="3">
+        <v>1000</v>
+      </c>
+      <c r="E51" s="3"/>
+      <c r="F51" s="3">
+        <v>10000</v>
+      </c>
+      <c r="G51" s="3"/>
+      <c r="H51" s="3">
+        <v>100000</v>
+      </c>
+      <c r="I51" s="3"/>
+      <c r="J51" s="3">
+        <v>1000000</v>
+      </c>
+      <c r="K51" s="3"/>
+      <c r="L51" s="3">
+        <v>10000000</v>
+      </c>
+      <c r="M51" s="3"/>
+    </row>
+    <row r="52" spans="4:14" x14ac:dyDescent="0.2">
+      <c r="D52" t="s">
+        <v>0</v>
+      </c>
+      <c r="E52" t="s">
+        <v>1</v>
+      </c>
+      <c r="F52" t="s">
+        <v>0</v>
+      </c>
+      <c r="G52" t="s">
+        <v>1</v>
+      </c>
+      <c r="H52" t="s">
+        <v>0</v>
+      </c>
+      <c r="I52" t="s">
+        <v>1</v>
+      </c>
+      <c r="J52" t="s">
+        <v>0</v>
+      </c>
+      <c r="K52" t="s">
+        <v>1</v>
+      </c>
+      <c r="L52" t="s">
+        <v>0</v>
+      </c>
+      <c r="M52" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="4:14" x14ac:dyDescent="0.2">
+      <c r="D53">
+        <v>9.8051700000000002E-3</v>
+      </c>
+      <c r="E53">
+        <v>6.0431699999999996E-3</v>
+      </c>
+      <c r="F53">
+        <v>5.3897199999999999E-2</v>
+      </c>
+      <c r="G53">
+        <v>2.35877E-2</v>
+      </c>
+      <c r="H53">
+        <v>0.26741900000000002</v>
+      </c>
+      <c r="I53">
+        <v>0.33307700000000001</v>
+      </c>
+      <c r="J53">
+        <v>2.2680199999999999</v>
+      </c>
+      <c r="K53">
+        <v>2.2116899999999999</v>
+      </c>
+      <c r="L53">
+        <v>24.868200000000002</v>
+      </c>
+      <c r="M53">
+        <v>23.525600000000001</v>
+      </c>
+      <c r="N53" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="54" spans="4:14" x14ac:dyDescent="0.2">
+      <c r="D54">
+        <v>1.9316599999999999E-4</v>
+      </c>
+      <c r="E54">
+        <v>1.7145800000000001E-4</v>
+      </c>
+      <c r="F54">
+        <v>1.0235400000000001E-3</v>
+      </c>
+      <c r="G54">
+        <v>1.1745799999999999E-3</v>
+      </c>
+      <c r="H54">
+        <v>7.2672500000000003E-3</v>
+      </c>
+      <c r="I54">
+        <v>3.1710200000000001E-2</v>
+      </c>
+      <c r="J54">
+        <v>0.10247299999999999</v>
+      </c>
+      <c r="K54">
+        <v>0.76694799999999996</v>
+      </c>
+      <c r="L54">
+        <v>0.93411900000000003</v>
+      </c>
+      <c r="M54">
+        <v>16.495000000000001</v>
+      </c>
+      <c r="N54" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="55" spans="4:14" x14ac:dyDescent="0.2">
+      <c r="D55">
+        <v>2.0491699999999999E-4</v>
+      </c>
+      <c r="E55">
+        <v>3.7733299999999999E-4</v>
+      </c>
+      <c r="F55">
+        <v>1.14533E-3</v>
+      </c>
+      <c r="G55">
+        <v>8.9375000000000001E-4</v>
+      </c>
+      <c r="H55">
+        <v>1.0344000000000001E-2</v>
+      </c>
+      <c r="I55">
+        <v>2.6686399999999999E-2</v>
+      </c>
+      <c r="J55">
+        <v>0.22517499999999999</v>
+      </c>
+      <c r="K55">
+        <v>0.27585799999999999</v>
+      </c>
+      <c r="L55">
+        <v>5.4665999999999997</v>
+      </c>
+      <c r="M55">
+        <v>3.8739400000000002</v>
+      </c>
+      <c r="N55" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="56" spans="4:14" x14ac:dyDescent="0.2">
+      <c r="D56">
+        <v>6.2521199999999999E-3</v>
+      </c>
+      <c r="E56">
+        <v>3.97125E-3</v>
+      </c>
+      <c r="F56">
+        <v>2.4501100000000001E-2</v>
+      </c>
+      <c r="G56">
+        <v>1.3133000000000001E-2</v>
+      </c>
+      <c r="H56">
+        <v>0.131468</v>
+      </c>
+      <c r="I56">
+        <v>0.13878099999999999</v>
+      </c>
+      <c r="J56">
+        <v>1.3029200000000001</v>
+      </c>
+      <c r="K56">
+        <v>1.7654700000000001</v>
+      </c>
+      <c r="L56">
+        <v>13.4763</v>
+      </c>
+      <c r="M56">
+        <v>27.3931</v>
+      </c>
+      <c r="N56" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="57" spans="4:14" x14ac:dyDescent="0.2">
+      <c r="D57">
+        <v>4.3512100000000003E-3</v>
+      </c>
+      <c r="E57">
+        <v>3.3080399999999999E-3</v>
+      </c>
+      <c r="F57">
+        <v>1.6129000000000001E-2</v>
+      </c>
+      <c r="G57">
+        <v>1.33826E-2</v>
+      </c>
+      <c r="H57">
+        <v>0.24635399999999999</v>
+      </c>
+      <c r="I57">
+        <v>0.14485999999999999</v>
+      </c>
+      <c r="J57">
+        <v>1.4527000000000001</v>
+      </c>
+      <c r="K57">
+        <v>1.5986400000000001</v>
+      </c>
+      <c r="L57">
+        <v>15.844099999999999</v>
+      </c>
+      <c r="M57">
+        <v>27.226199999999999</v>
+      </c>
+      <c r="N57" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="58" spans="4:14" x14ac:dyDescent="0.2">
+      <c r="D58">
+        <v>2.08723E-2</v>
+      </c>
+      <c r="E58">
+        <v>1.39217E-2</v>
+      </c>
+      <c r="F58">
+        <v>9.6760700000000005E-2</v>
+      </c>
+      <c r="G58">
+        <v>5.22076E-2</v>
+      </c>
+      <c r="H58">
+        <v>0.66292499999999999</v>
+      </c>
+      <c r="I58">
+        <v>0.67520400000000003</v>
+      </c>
+      <c r="J58">
+        <v>5.3513799999999998</v>
+      </c>
+      <c r="K58">
+        <v>6.6186800000000003</v>
+      </c>
+      <c r="L58">
+        <v>60.589799999999997</v>
+      </c>
+      <c r="M58">
+        <v>98.513900000000007</v>
+      </c>
+      <c r="N58" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="11">
-    <mergeCell ref="J3:K3"/>
-    <mergeCell ref="L3:M3"/>
-    <mergeCell ref="D2:M2"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="L4:M4"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="H3:I3"/>
+  <mergeCells count="33">
+    <mergeCell ref="D46:M46"/>
+    <mergeCell ref="D49:M49"/>
+    <mergeCell ref="D50:M50"/>
+    <mergeCell ref="D51:E51"/>
+    <mergeCell ref="F51:G51"/>
+    <mergeCell ref="H51:I51"/>
+    <mergeCell ref="J51:K51"/>
+    <mergeCell ref="L51:M51"/>
+    <mergeCell ref="D23:M23"/>
+    <mergeCell ref="D36:M36"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="F38:G38"/>
+    <mergeCell ref="H38:I38"/>
+    <mergeCell ref="J38:K38"/>
+    <mergeCell ref="L38:M38"/>
+    <mergeCell ref="D24:M24"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="H25:I25"/>
+    <mergeCell ref="J25:K25"/>
+    <mergeCell ref="L25:M25"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="L7:M7"/>
+    <mergeCell ref="D6:M6"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="J8:K8"/>
+    <mergeCell ref="L8:M8"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="D37:M37"/>
   </mergeCells>
-  <conditionalFormatting sqref="D6:D11">
-    <cfRule type="colorScale" priority="6">
+  <conditionalFormatting sqref="D10:D15">
+    <cfRule type="colorScale" priority="11">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -795,7 +1720,31 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D6:M11">
+  <conditionalFormatting sqref="D8:M8">
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D10:M15">
+    <cfRule type="colorScale" priority="9">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D27:M32">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
@@ -807,7 +1756,31 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D4:M4">
+  <conditionalFormatting sqref="D40:M45">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D40:K45">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D53:M58">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>